<commit_message>
change to raptor.c; added functions to set clock using int and ext osc
</commit_message>
<xml_diff>
--- a/hardware/raptor.xlsx
+++ b/hardware/raptor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeffdi/Projects/raptor/hardware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{711EF31D-F1AF-7B4E-8520-139EE39D3DFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{309EB436-5B45-824B-A807-63064A3FD1B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-31220" yWindow="3400" windowWidth="23280" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="160">
   <si>
     <t>Reference</t>
   </si>
@@ -240,9 +240,6 @@
     <t>Digikey PN</t>
   </si>
   <si>
-    <t>Part Page</t>
-  </si>
-  <si>
     <t>LMF107B7104KAHT</t>
   </si>
   <si>
@@ -492,9 +489,6 @@
     <t>CSTCR6M25G55B-R0</t>
   </si>
   <si>
-    <t>stocked at mousser</t>
-  </si>
-  <si>
     <t>U3</t>
   </si>
   <si>
@@ -513,7 +507,7 @@
     <t>296-37177-1-ND</t>
   </si>
   <si>
-    <t>dni</t>
+    <t>Link</t>
   </si>
 </sst>
 </file>
@@ -1392,7 +1386,7 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD29"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21"/>
@@ -1427,7 +1421,7 @@
         <v>69</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>70</v>
+        <v>159</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>3</v>
@@ -1444,16 +1438,16 @@
         <v>5</v>
       </c>
       <c r="D2" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="F2" s="8" t="s">
+      <c r="G2" s="4" t="s">
         <v>139</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>140</v>
       </c>
       <c r="H2" t="s">
         <v>6</v>
@@ -1470,16 +1464,16 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" t="s">
         <v>71</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>72</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>74</v>
       </c>
       <c r="H3" t="s">
         <v>6</v>
@@ -1496,16 +1490,16 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F4" t="s">
         <v>75</v>
       </c>
-      <c r="E4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="G4" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>77</v>
       </c>
       <c r="H4" t="s">
         <v>6</v>
@@ -1522,16 +1516,16 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E5" t="s">
         <v>82</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>83</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>85</v>
       </c>
       <c r="H5" t="s">
         <v>13</v>
@@ -1548,16 +1542,16 @@
         <v>15</v>
       </c>
       <c r="D6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" t="s">
         <v>78</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>79</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" s="4" t="s">
         <v>80</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>81</v>
       </c>
       <c r="H6" t="s">
         <v>16</v>
@@ -1574,10 +1568,10 @@
         <v>18</v>
       </c>
       <c r="D7" t="s">
+        <v>135</v>
+      </c>
+      <c r="E7" t="s">
         <v>136</v>
-      </c>
-      <c r="E7" t="s">
-        <v>137</v>
       </c>
       <c r="H7" t="s">
         <v>19</v>
@@ -1594,16 +1588,16 @@
         <v>21</v>
       </c>
       <c r="D8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E8" t="s">
         <v>86</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>87</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" s="4" t="s">
         <v>88</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>89</v>
       </c>
       <c r="H8" t="s">
         <v>22</v>
@@ -1620,16 +1614,16 @@
         <v>24</v>
       </c>
       <c r="D9" t="s">
+        <v>89</v>
+      </c>
+      <c r="E9" t="s">
         <v>90</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>91</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" s="4" t="s">
         <v>92</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>93</v>
       </c>
       <c r="H9" t="s">
         <v>25</v>
@@ -1646,16 +1640,16 @@
         <v>27</v>
       </c>
       <c r="D10" t="s">
+        <v>93</v>
+      </c>
+      <c r="E10" t="s">
+        <v>90</v>
+      </c>
+      <c r="F10" t="s">
         <v>94</v>
       </c>
-      <c r="E10" t="s">
-        <v>91</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="G10" s="4" t="s">
         <v>95</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>96</v>
       </c>
       <c r="H10" t="s">
         <v>28</v>
@@ -1675,10 +1669,10 @@
         <v>32</v>
       </c>
       <c r="F11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H11" t="s">
         <v>31</v>
@@ -1695,16 +1689,16 @@
         <v>34</v>
       </c>
       <c r="D12" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E12" t="s">
+        <v>82</v>
+      </c>
+      <c r="F12" t="s">
         <v>100</v>
       </c>
-      <c r="E12" t="s">
-        <v>83</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="G12" s="4" t="s">
         <v>101</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>102</v>
       </c>
       <c r="H12" t="s">
         <v>35</v>
@@ -1714,23 +1708,23 @@
       <c r="A13" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>161</v>
+      <c r="B13" s="1">
+        <v>0</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>37</v>
       </c>
       <c r="D13" t="s">
+        <v>140</v>
+      </c>
+      <c r="E13" t="s">
         <v>141</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>142</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" s="4" t="s">
         <v>143</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>144</v>
       </c>
       <c r="H13" t="s">
         <v>38</v>
@@ -1740,23 +1734,23 @@
       <c r="A14" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>161</v>
+      <c r="B14" s="1">
+        <v>0</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>40</v>
       </c>
       <c r="D14" t="s">
+        <v>148</v>
+      </c>
+      <c r="E14" t="s">
+        <v>141</v>
+      </c>
+      <c r="F14" t="s">
         <v>149</v>
       </c>
-      <c r="E14" t="s">
-        <v>142</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="G14" s="4" t="s">
         <v>150</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>151</v>
       </c>
       <c r="H14" t="s">
         <v>41</v>
@@ -1766,23 +1760,23 @@
       <c r="A15" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>161</v>
+      <c r="B15" s="1">
+        <v>0</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>43</v>
       </c>
       <c r="D15" t="s">
+        <v>144</v>
+      </c>
+      <c r="E15" t="s">
         <v>145</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>146</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" s="4" t="s">
         <v>147</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>148</v>
       </c>
       <c r="H15" t="s">
         <v>44</v>
@@ -1799,16 +1793,16 @@
         <v>46</v>
       </c>
       <c r="D16" t="s">
+        <v>102</v>
+      </c>
+      <c r="E16" t="s">
         <v>103</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>104</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" s="4" t="s">
         <v>105</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>106</v>
       </c>
       <c r="H16" t="s">
         <v>47</v>
@@ -1825,16 +1819,16 @@
         <v>150</v>
       </c>
       <c r="D17" t="s">
+        <v>106</v>
+      </c>
+      <c r="E17" t="s">
         <v>107</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>108</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" s="4" t="s">
         <v>109</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>110</v>
       </c>
       <c r="H17" t="s">
         <v>47</v>
@@ -1851,16 +1845,16 @@
         <v>50</v>
       </c>
       <c r="D18" t="s">
+        <v>102</v>
+      </c>
+      <c r="E18" t="s">
         <v>103</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>104</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" s="4" t="s">
         <v>105</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>106</v>
       </c>
       <c r="H18" t="s">
         <v>47</v>
@@ -1877,16 +1871,16 @@
         <v>0</v>
       </c>
       <c r="D19" t="s">
+        <v>110</v>
+      </c>
+      <c r="E19" t="s">
+        <v>103</v>
+      </c>
+      <c r="F19" t="s">
         <v>111</v>
       </c>
-      <c r="E19" t="s">
-        <v>104</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="G19" s="4" t="s">
         <v>112</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>113</v>
       </c>
       <c r="H19" t="s">
         <v>47</v>
@@ -1903,16 +1897,16 @@
         <v>53</v>
       </c>
       <c r="D20" t="s">
+        <v>113</v>
+      </c>
+      <c r="E20" t="s">
+        <v>103</v>
+      </c>
+      <c r="F20" t="s">
         <v>114</v>
       </c>
-      <c r="E20" t="s">
-        <v>104</v>
-      </c>
-      <c r="F20" t="s">
+      <c r="G20" s="4" t="s">
         <v>115</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>116</v>
       </c>
       <c r="H20" t="s">
         <v>47</v>
@@ -1929,16 +1923,16 @@
         <v>55</v>
       </c>
       <c r="D21" t="s">
+        <v>116</v>
+      </c>
+      <c r="E21" t="s">
+        <v>103</v>
+      </c>
+      <c r="F21" t="s">
         <v>117</v>
       </c>
-      <c r="E21" t="s">
-        <v>104</v>
-      </c>
-      <c r="F21" t="s">
+      <c r="G21" s="4" t="s">
         <v>118</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>119</v>
       </c>
       <c r="H21" t="s">
         <v>47</v>
@@ -1955,16 +1949,16 @@
         <v>57</v>
       </c>
       <c r="D22" t="s">
+        <v>119</v>
+      </c>
+      <c r="E22" t="s">
         <v>120</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>121</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" s="4" t="s">
         <v>122</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>123</v>
       </c>
       <c r="H22" t="s">
         <v>58</v>
@@ -1981,16 +1975,16 @@
         <v>60</v>
       </c>
       <c r="D23" t="s">
+        <v>123</v>
+      </c>
+      <c r="E23" t="s">
+        <v>90</v>
+      </c>
+      <c r="F23" t="s">
         <v>124</v>
       </c>
-      <c r="E23" t="s">
-        <v>91</v>
-      </c>
-      <c r="F23" t="s">
+      <c r="G23" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>126</v>
       </c>
       <c r="H23" t="s">
         <v>25</v>
@@ -2007,16 +2001,16 @@
         <v>62</v>
       </c>
       <c r="D24" t="s">
+        <v>126</v>
+      </c>
+      <c r="E24" t="s">
         <v>127</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>128</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" s="4" t="s">
         <v>129</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>130</v>
       </c>
       <c r="H24" t="s">
         <v>63</v>
@@ -2024,51 +2018,51 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B25" s="1">
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E25" t="s">
         <v>32</v>
       </c>
       <c r="F25" t="s">
+        <v>97</v>
+      </c>
+      <c r="G25" s="4" t="s">
         <v>98</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B26" s="1">
         <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E26" t="s">
         <v>32</v>
       </c>
       <c r="F26" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G26" s="4"/>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B27" s="1">
         <v>1</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D27" t="s">
         <v>64</v>
@@ -2077,10 +2071,10 @@
         <v>66</v>
       </c>
       <c r="F27" t="s">
+        <v>132</v>
+      </c>
+      <c r="G27" s="4" t="s">
         <v>133</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>134</v>
       </c>
       <c r="H27" t="s">
         <v>65</v>
@@ -2088,22 +2082,19 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B28" s="1">
         <v>1</v>
       </c>
       <c r="C28" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D28" t="s">
         <v>152</v>
-      </c>
-      <c r="D28" t="s">
-        <v>153</v>
       </c>
       <c r="E28" t="s">
         <v>66</v>
-      </c>
-      <c r="G28" t="s">
-        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>